<commit_message>
new R version defaults caused errors with minke data load
default now to load "long" numbers as character, breaking an example
</commit_message>
<xml_diff>
--- a/inst/minke.xlsx
+++ b/inst/minke.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="23955" windowHeight="12075"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="23960" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -57,8 +62,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,13 +368,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="8.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,14 +387,14 @@
       <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>86.75</v>
       </c>
       <c r="E1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -395,14 +404,14 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>86.75</v>
       </c>
       <c r="E2">
         <v>0.22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -412,14 +421,14 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>86.75</v>
       </c>
       <c r="E3">
         <v>0.16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -429,14 +438,14 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>86.75</v>
       </c>
       <c r="E4">
         <v>0.78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -446,14 +455,14 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>86.75</v>
       </c>
       <c r="E5">
         <v>0.21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -463,14 +472,14 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>86.75</v>
       </c>
       <c r="E6">
         <v>0.95</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -480,14 +489,14 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>10.57</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -497,14 +506,14 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>10.57</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -514,14 +523,14 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>10.57</v>
       </c>
       <c r="E9">
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -531,14 +540,14 @@
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>10.57</v>
       </c>
       <c r="E10">
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -548,14 +557,14 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>10.57</v>
       </c>
       <c r="E11">
         <v>0.93</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -565,14 +574,14 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>10.57</v>
       </c>
       <c r="E12">
         <v>0.38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -582,14 +591,14 @@
       <c r="C13">
         <v>3</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>16.57</v>
       </c>
       <c r="E13">
         <v>0.39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -599,14 +608,14 @@
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>16.57</v>
       </c>
       <c r="E14">
         <v>0.61</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -616,14 +625,14 @@
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>16.57</v>
       </c>
       <c r="E15">
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -633,14 +642,14 @@
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>113.13</v>
       </c>
       <c r="E16">
         <v>0.34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -650,14 +659,14 @@
       <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>113.13</v>
       </c>
       <c r="E17">
         <v>0.52</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -667,14 +676,14 @@
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>113.13</v>
       </c>
       <c r="E18">
         <v>0.36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -684,14 +693,14 @@
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>113.13</v>
       </c>
       <c r="E19">
         <v>1.22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -701,14 +710,14 @@
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>113.13</v>
       </c>
       <c r="E20">
         <v>0.68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -718,14 +727,14 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>113.13</v>
       </c>
       <c r="E21">
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -735,14 +744,14 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>113.13</v>
       </c>
       <c r="E22">
         <v>0.26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -752,14 +761,14 @@
       <c r="C23">
         <v>4</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>113.13</v>
       </c>
       <c r="E23">
         <v>1.21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -769,14 +778,14 @@
       <c r="C24">
         <v>4</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>113.13</v>
       </c>
       <c r="E24">
         <v>0.52</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -786,11 +795,11 @@
       <c r="C25">
         <v>5</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>15.07</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -800,11 +809,11 @@
       <c r="C26">
         <v>6</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>9.9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -814,14 +823,14 @@
       <c r="C27">
         <v>7</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>25.71</v>
       </c>
       <c r="E27">
         <v>0.18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -831,14 +840,14 @@
       <c r="C28">
         <v>7</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>25.71</v>
       </c>
       <c r="E28">
         <v>0.36</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -848,14 +857,14 @@
       <c r="C29">
         <v>7</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>25.71</v>
       </c>
       <c r="E29">
         <v>0.61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -865,14 +874,14 @@
       <c r="C30">
         <v>7</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>25.71</v>
       </c>
       <c r="E30">
         <v>0.61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -882,14 +891,14 @@
       <c r="C31">
         <v>8</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>57.55</v>
       </c>
       <c r="E31">
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -899,14 +908,14 @@
       <c r="C32">
         <v>8</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>57.55</v>
       </c>
       <c r="E32">
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -916,11 +925,11 @@
       <c r="C33">
         <v>9</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>7.67</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -930,11 +939,11 @@
       <c r="C34">
         <v>10</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>13.02</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -944,11 +953,11 @@
       <c r="C35">
         <v>11</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>52.65</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -958,11 +967,11 @@
       <c r="C36">
         <v>12</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>0.19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -972,14 +981,14 @@
       <c r="C37">
         <v>13</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>75.63</v>
       </c>
       <c r="E37">
         <v>0.1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -989,14 +998,14 @@
       <c r="C38">
         <v>13</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>75.63</v>
       </c>
       <c r="E38">
         <v>0.68</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -1006,14 +1015,14 @@
       <c r="C39">
         <v>13</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>75.63</v>
       </c>
       <c r="E39">
         <v>0.31</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1023,14 +1032,14 @@
       <c r="C40">
         <v>13</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>75.63</v>
       </c>
       <c r="E40">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1040,14 +1049,14 @@
       <c r="C41">
         <v>13</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>75.63</v>
       </c>
       <c r="E41">
         <v>0.49</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1057,14 +1066,14 @@
       <c r="C42">
         <v>13</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>75.63</v>
       </c>
       <c r="E42">
         <v>0.46</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1074,14 +1083,14 @@
       <c r="C43">
         <v>13</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>75.63</v>
       </c>
       <c r="E43">
         <v>0.36</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1091,14 +1100,14 @@
       <c r="C44">
         <v>13</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>75.63</v>
       </c>
       <c r="E44">
         <v>0.09</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1108,14 +1117,14 @@
       <c r="C45">
         <v>13</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>75.63</v>
       </c>
       <c r="E45">
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1125,14 +1134,14 @@
       <c r="C46">
         <v>14</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>83.33</v>
       </c>
       <c r="E46">
         <v>0.49</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -1142,14 +1151,14 @@
       <c r="C47">
         <v>14</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>83.33</v>
       </c>
       <c r="E47">
         <v>1.94</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1159,14 +1168,14 @@
       <c r="C48">
         <v>14</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>83.33</v>
       </c>
       <c r="E48">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -1176,14 +1185,14 @@
       <c r="C49">
         <v>14</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>83.33</v>
       </c>
       <c r="E49">
         <v>0.85</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -1193,14 +1202,14 @@
       <c r="C50">
         <v>14</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>83.33</v>
       </c>
       <c r="E50">
         <v>0.63</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -1210,14 +1219,14 @@
       <c r="C51">
         <v>14</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>83.33</v>
       </c>
       <c r="E51">
         <v>0.39</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -1227,14 +1236,14 @@
       <c r="C52">
         <v>14</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>83.33</v>
       </c>
       <c r="E52">
         <v>0.65</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -1244,14 +1253,14 @@
       <c r="C53">
         <v>14</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>83.33</v>
       </c>
       <c r="E53">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1261,14 +1270,14 @@
       <c r="C54">
         <v>14</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>83.33</v>
       </c>
       <c r="E54">
         <v>0.91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -1278,14 +1287,14 @@
       <c r="C55">
         <v>14</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>83.33</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -1295,14 +1304,14 @@
       <c r="C56">
         <v>14</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>83.33</v>
       </c>
       <c r="E56">
         <v>1.18</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1312,14 +1321,14 @@
       <c r="C57">
         <v>15</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>100.93</v>
       </c>
       <c r="E57">
         <v>0.1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1329,14 +1338,14 @@
       <c r="C58">
         <v>15</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>100.93</v>
       </c>
       <c r="E58">
         <v>0.37</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -1346,14 +1355,14 @@
       <c r="C59">
         <v>15</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>100.93</v>
       </c>
       <c r="E59">
         <v>0.59</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -1363,14 +1372,14 @@
       <c r="C60">
         <v>15</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="1">
         <v>100.93</v>
       </c>
       <c r="E60">
         <v>0.45</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -1380,14 +1389,14 @@
       <c r="C61">
         <v>15</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>100.93</v>
       </c>
       <c r="E61">
         <v>0.53</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -1397,14 +1406,14 @@
       <c r="C62">
         <v>16</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
         <v>110.55</v>
       </c>
       <c r="E62">
         <v>0.21</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -1414,11 +1423,11 @@
       <c r="C63">
         <v>17</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>97.5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -1428,14 +1437,14 @@
       <c r="C64">
         <v>18</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
         <v>126.32</v>
       </c>
       <c r="E64">
         <v>0.85</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -1445,14 +1454,14 @@
       <c r="C65">
         <v>18</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="1">
         <v>126.32</v>
       </c>
       <c r="E65">
         <v>1.48</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -1462,14 +1471,14 @@
       <c r="C66">
         <v>18</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>126.32</v>
       </c>
       <c r="E66">
         <v>1.44</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -1479,14 +1488,14 @@
       <c r="C67">
         <v>18</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="1">
         <v>126.32</v>
       </c>
       <c r="E67">
         <v>0.9</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -1496,14 +1505,14 @@
       <c r="C68">
         <v>18</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>126.32</v>
       </c>
       <c r="E68">
         <v>0.01</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -1513,14 +1522,14 @@
       <c r="C69">
         <v>18</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="1">
         <v>126.32</v>
       </c>
       <c r="E69">
         <v>1.58</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -1530,14 +1539,14 @@
       <c r="C70">
         <v>18</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>126.32</v>
       </c>
       <c r="E70">
         <v>0.68</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -1547,14 +1556,14 @@
       <c r="C71">
         <v>18</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>126.32</v>
       </c>
       <c r="E71">
         <v>0.8</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -1564,14 +1573,14 @@
       <c r="C72">
         <v>18</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
         <v>126.32</v>
       </c>
       <c r="E72">
         <v>0.64</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -1581,14 +1590,14 @@
       <c r="C73">
         <v>18</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="1">
         <v>126.32</v>
       </c>
       <c r="E73">
         <v>1.45</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -1598,14 +1607,14 @@
       <c r="C74">
         <v>18</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>126.32</v>
       </c>
       <c r="E74">
         <v>0.31</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -1615,14 +1624,14 @@
       <c r="C75">
         <v>18</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="1">
         <v>126.32</v>
       </c>
       <c r="E75">
         <v>0.31</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -1632,14 +1641,14 @@
       <c r="C76">
         <v>18</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="1">
         <v>126.32</v>
       </c>
       <c r="E76">
         <v>0.85</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -1649,14 +1658,14 @@
       <c r="C77">
         <v>18</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="1">
         <v>126.32</v>
       </c>
       <c r="E77">
         <v>0.49</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -1666,14 +1675,14 @@
       <c r="C78">
         <v>18</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="1">
         <v>126.32</v>
       </c>
       <c r="E78">
         <v>0.67</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -1683,14 +1692,14 @@
       <c r="C79">
         <v>18</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="1">
         <v>126.32</v>
       </c>
       <c r="E79">
         <v>0.27</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>1</v>
       </c>
@@ -1700,14 +1709,14 @@
       <c r="C80">
         <v>18</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>126.32</v>
       </c>
       <c r="E80">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -1717,14 +1726,14 @@
       <c r="C81">
         <v>18</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="1">
         <v>126.32</v>
       </c>
       <c r="E81">
         <v>0.23</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -1734,14 +1743,14 @@
       <c r="C82">
         <v>19</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="1">
         <v>99.37</v>
       </c>
       <c r="E82">
         <v>0.39</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -1751,14 +1760,14 @@
       <c r="C83">
         <v>20</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
         <v>137.38999999999999</v>
       </c>
       <c r="E83">
         <v>1.17</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -1768,14 +1777,14 @@
       <c r="C84">
         <v>20</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>137.38999999999999</v>
       </c>
       <c r="E84">
         <v>0.97</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -1785,14 +1794,14 @@
       <c r="C85">
         <v>21</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="1">
         <v>106.76</v>
       </c>
       <c r="E85">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -1802,14 +1811,14 @@
       <c r="C86">
         <v>21</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>106.76</v>
       </c>
       <c r="E86">
         <v>0.59</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -1819,14 +1828,14 @@
       <c r="C87">
         <v>21</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="1">
         <v>106.76</v>
       </c>
       <c r="E87">
         <v>1.01</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>1</v>
       </c>
@@ -1836,14 +1845,14 @@
       <c r="C88">
         <v>21</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
         <v>106.76</v>
       </c>
       <c r="E88">
         <v>0.87</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -1853,14 +1862,14 @@
       <c r="C89">
         <v>21</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
         <v>106.76</v>
       </c>
       <c r="E89">
         <v>0.13</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -1870,14 +1879,14 @@
       <c r="C90">
         <v>21</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="1">
         <v>106.76</v>
       </c>
       <c r="E90">
         <v>0.78</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -1887,14 +1896,14 @@
       <c r="C91">
         <v>22</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="1">
         <v>113.28</v>
       </c>
       <c r="E91">
         <v>0.97</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -1904,14 +1913,14 @@
       <c r="C92">
         <v>22</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="1">
         <v>113.28</v>
       </c>
       <c r="E92">
         <v>0.48</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>1</v>
       </c>
@@ -1921,11 +1930,11 @@
       <c r="C93">
         <v>23</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="1">
         <v>144.9</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>1</v>
       </c>
@@ -1935,14 +1944,14 @@
       <c r="C94">
         <v>24</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="1">
         <v>130.33000000000001</v>
       </c>
       <c r="E94">
         <v>0.41</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -1952,14 +1961,14 @@
       <c r="C95">
         <v>24</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="1">
         <v>130.33000000000001</v>
       </c>
       <c r="E95">
         <v>0.15</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -1969,14 +1978,14 @@
       <c r="C96">
         <v>24</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="1">
         <v>130.33000000000001</v>
       </c>
       <c r="E96">
         <v>0.09</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -1986,14 +1995,14 @@
       <c r="C97">
         <v>24</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="1">
         <v>130.33000000000001</v>
       </c>
       <c r="E97">
         <v>0.1</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>1</v>
       </c>
@@ -2003,14 +2012,14 @@
       <c r="C98">
         <v>24</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="1">
         <v>130.33000000000001</v>
       </c>
       <c r="E98">
         <v>0.1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -2020,12 +2029,17 @@
       <c r="C99">
         <v>25</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="1">
         <v>107.72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2035,9 +2049,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2047,8 +2066,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>